<commit_message>
LMK's boutons for D01 and D05
</commit_message>
<xml_diff>
--- a/excel_output/XRZCT_objects.xlsx
+++ b/excel_output/XRZCT_objects.xlsx
@@ -1,27 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dusten Hubbard\Dropbox\GitHub\XRZCT\spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dusten Hubbard\Dropbox\GitHub\XRZCT\excel_output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85AC4688-78DA-4946-B8EA-58718771BA93}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F931D9-FA86-4869-84AE-7E9A78D21C04}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="objects" sheetId="1" r:id="rId1"/>
     <sheet name="d01" sheetId="2" r:id="rId2"/>
+    <sheet name="d02" sheetId="3" r:id="rId3"/>
+    <sheet name="d05" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3745" uniqueCount="3575">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4024" uniqueCount="3575">
   <si>
     <t>Object</t>
   </si>
@@ -11597,8 +11599,8 @@
   <dimension ref="A1:G3569"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -93708,7 +93710,7 @@
   <dimension ref="A1:N54"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -95908,10 +95910,3529 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D27">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D27">
     <sortCondition ref="B2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B59CBA1-CE7F-4638-A5AF-A1EF37FB9AAD}">
+  <dimension ref="A1:T50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:O1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>598</v>
+      </c>
+      <c r="R1">
+        <v>1</v>
+      </c>
+      <c r="S1">
+        <v>204</v>
+      </c>
+      <c r="T1">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>818</v>
+      </c>
+      <c r="B2">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>819</v>
+      </c>
+      <c r="B3">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>820</v>
+      </c>
+      <c r="B4">
+        <v>14</v>
+      </c>
+      <c r="C4">
+        <v>17</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>713</v>
+      </c>
+      <c r="G4">
+        <v>16</v>
+      </c>
+      <c r="H4">
+        <v>17</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="K4" t="s">
+        <v>771</v>
+      </c>
+      <c r="L4">
+        <v>16</v>
+      </c>
+      <c r="M4">
+        <v>17</v>
+      </c>
+      <c r="N4">
+        <v>3</v>
+      </c>
+      <c r="O4">
+        <v>0.12812599999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>822</v>
+      </c>
+      <c r="B5">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <v>26</v>
+      </c>
+      <c r="D5">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>714</v>
+      </c>
+      <c r="G5">
+        <v>28</v>
+      </c>
+      <c r="H5">
+        <v>41</v>
+      </c>
+      <c r="I5">
+        <v>24</v>
+      </c>
+      <c r="K5" t="s">
+        <v>772</v>
+      </c>
+      <c r="L5">
+        <v>28</v>
+      </c>
+      <c r="M5">
+        <v>41</v>
+      </c>
+      <c r="N5">
+        <v>24</v>
+      </c>
+      <c r="O5">
+        <v>0.63951499999999994</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>824</v>
+      </c>
+      <c r="B6">
+        <v>26</v>
+      </c>
+      <c r="C6">
+        <v>31</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="F6" t="s">
+        <v>715</v>
+      </c>
+      <c r="G6">
+        <v>31</v>
+      </c>
+      <c r="H6">
+        <v>36</v>
+      </c>
+      <c r="I6">
+        <v>6</v>
+      </c>
+      <c r="K6" t="s">
+        <v>773</v>
+      </c>
+      <c r="L6">
+        <v>31</v>
+      </c>
+      <c r="M6">
+        <v>36</v>
+      </c>
+      <c r="N6">
+        <v>6</v>
+      </c>
+      <c r="O6">
+        <v>8.47445E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>826</v>
+      </c>
+      <c r="B7">
+        <v>31</v>
+      </c>
+      <c r="C7">
+        <v>37</v>
+      </c>
+      <c r="D7">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>716</v>
+      </c>
+      <c r="G7">
+        <v>26</v>
+      </c>
+      <c r="H7">
+        <v>29</v>
+      </c>
+      <c r="I7">
+        <v>4</v>
+      </c>
+      <c r="K7" t="s">
+        <v>774</v>
+      </c>
+      <c r="L7">
+        <v>26</v>
+      </c>
+      <c r="M7">
+        <v>29</v>
+      </c>
+      <c r="N7">
+        <v>4</v>
+      </c>
+      <c r="O7">
+        <v>3.9960500000000003E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>828</v>
+      </c>
+      <c r="B8">
+        <v>41</v>
+      </c>
+      <c r="C8">
+        <v>47</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>717</v>
+      </c>
+      <c r="G8">
+        <v>36</v>
+      </c>
+      <c r="H8">
+        <v>38</v>
+      </c>
+      <c r="I8">
+        <v>3</v>
+      </c>
+      <c r="K8" t="s">
+        <v>775</v>
+      </c>
+      <c r="L8">
+        <v>36</v>
+      </c>
+      <c r="M8">
+        <v>38</v>
+      </c>
+      <c r="N8">
+        <v>3</v>
+      </c>
+      <c r="O8">
+        <v>3.1502700000000002E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>830</v>
+      </c>
+      <c r="B9">
+        <v>46</v>
+      </c>
+      <c r="C9">
+        <v>48</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>718</v>
+      </c>
+      <c r="G9">
+        <v>31</v>
+      </c>
+      <c r="H9">
+        <v>36</v>
+      </c>
+      <c r="I9">
+        <v>6</v>
+      </c>
+      <c r="K9" t="s">
+        <v>776</v>
+      </c>
+      <c r="L9">
+        <v>31</v>
+      </c>
+      <c r="M9">
+        <v>36</v>
+      </c>
+      <c r="N9">
+        <v>6</v>
+      </c>
+      <c r="O9">
+        <v>9.9415100000000006E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>831</v>
+      </c>
+      <c r="B10">
+        <v>48</v>
+      </c>
+      <c r="C10">
+        <v>49</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>719</v>
+      </c>
+      <c r="G10">
+        <v>70</v>
+      </c>
+      <c r="H10">
+        <v>73</v>
+      </c>
+      <c r="I10">
+        <v>4</v>
+      </c>
+      <c r="K10" t="s">
+        <v>777</v>
+      </c>
+      <c r="L10">
+        <v>70</v>
+      </c>
+      <c r="M10">
+        <v>73</v>
+      </c>
+      <c r="N10">
+        <v>4</v>
+      </c>
+      <c r="O10">
+        <v>3.9379600000000001E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>833</v>
+      </c>
+      <c r="B11">
+        <v>49</v>
+      </c>
+      <c r="C11">
+        <v>53</v>
+      </c>
+      <c r="D11">
+        <v>5</v>
+      </c>
+      <c r="F11" t="s">
+        <v>720</v>
+      </c>
+      <c r="G11">
+        <v>50</v>
+      </c>
+      <c r="H11">
+        <v>53</v>
+      </c>
+      <c r="I11">
+        <v>4</v>
+      </c>
+      <c r="K11" t="s">
+        <v>778</v>
+      </c>
+      <c r="L11">
+        <v>50</v>
+      </c>
+      <c r="M11">
+        <v>53</v>
+      </c>
+      <c r="N11">
+        <v>5</v>
+      </c>
+      <c r="O11">
+        <v>7.6623899999999995E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>835</v>
+      </c>
+      <c r="B12">
+        <v>56</v>
+      </c>
+      <c r="C12">
+        <v>60</v>
+      </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="F12" t="s">
+        <v>721</v>
+      </c>
+      <c r="G12">
+        <v>71</v>
+      </c>
+      <c r="H12">
+        <v>73</v>
+      </c>
+      <c r="I12">
+        <v>3</v>
+      </c>
+      <c r="K12" t="s">
+        <v>779</v>
+      </c>
+      <c r="L12">
+        <v>71</v>
+      </c>
+      <c r="M12">
+        <v>73</v>
+      </c>
+      <c r="N12">
+        <v>3</v>
+      </c>
+      <c r="O12">
+        <v>3.8674100000000003E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>837</v>
+      </c>
+      <c r="B13">
+        <v>60</v>
+      </c>
+      <c r="C13">
+        <v>62</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="F13" t="s">
+        <v>722</v>
+      </c>
+      <c r="G13">
+        <v>71</v>
+      </c>
+      <c r="H13">
+        <v>72</v>
+      </c>
+      <c r="I13">
+        <v>2</v>
+      </c>
+      <c r="K13" t="s">
+        <v>780</v>
+      </c>
+      <c r="L13">
+        <v>71</v>
+      </c>
+      <c r="M13">
+        <v>72</v>
+      </c>
+      <c r="N13">
+        <v>3</v>
+      </c>
+      <c r="O13">
+        <v>5.7613299999999999E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>839</v>
+      </c>
+      <c r="B14">
+        <v>62</v>
+      </c>
+      <c r="C14">
+        <v>66</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+      <c r="F14" t="s">
+        <v>723</v>
+      </c>
+      <c r="G14">
+        <v>42</v>
+      </c>
+      <c r="H14">
+        <v>43</v>
+      </c>
+      <c r="I14">
+        <v>2</v>
+      </c>
+      <c r="K14" t="s">
+        <v>781</v>
+      </c>
+      <c r="L14">
+        <v>42</v>
+      </c>
+      <c r="M14">
+        <v>43</v>
+      </c>
+      <c r="N14">
+        <v>3</v>
+      </c>
+      <c r="O14">
+        <v>5.2319999999999998E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>841</v>
+      </c>
+      <c r="B15">
+        <v>63</v>
+      </c>
+      <c r="C15">
+        <v>71</v>
+      </c>
+      <c r="D15">
+        <v>9</v>
+      </c>
+      <c r="F15" t="s">
+        <v>724</v>
+      </c>
+      <c r="G15">
+        <v>63</v>
+      </c>
+      <c r="H15">
+        <v>71</v>
+      </c>
+      <c r="I15">
+        <v>9</v>
+      </c>
+      <c r="K15" t="s">
+        <v>782</v>
+      </c>
+      <c r="L15">
+        <v>63</v>
+      </c>
+      <c r="M15">
+        <v>71</v>
+      </c>
+      <c r="N15">
+        <v>9</v>
+      </c>
+      <c r="O15">
+        <v>0.35264299999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>842</v>
+      </c>
+      <c r="B16">
+        <v>67</v>
+      </c>
+      <c r="C16">
+        <v>68</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>844</v>
+      </c>
+      <c r="B17">
+        <v>70</v>
+      </c>
+      <c r="C17">
+        <v>72</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="F17" t="s">
+        <v>725</v>
+      </c>
+      <c r="G17">
+        <v>65</v>
+      </c>
+      <c r="H17">
+        <v>68</v>
+      </c>
+      <c r="I17">
+        <v>4</v>
+      </c>
+      <c r="K17" t="s">
+        <v>783</v>
+      </c>
+      <c r="L17">
+        <v>65</v>
+      </c>
+      <c r="M17">
+        <v>68</v>
+      </c>
+      <c r="N17">
+        <v>4</v>
+      </c>
+      <c r="O17">
+        <v>5.2469300000000003E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>846</v>
+      </c>
+      <c r="B18">
+        <v>78</v>
+      </c>
+      <c r="C18">
+        <v>81</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+      <c r="F18" t="s">
+        <v>726</v>
+      </c>
+      <c r="G18">
+        <v>55</v>
+      </c>
+      <c r="H18">
+        <v>56</v>
+      </c>
+      <c r="I18">
+        <v>2</v>
+      </c>
+      <c r="K18" t="s">
+        <v>784</v>
+      </c>
+      <c r="L18">
+        <v>55</v>
+      </c>
+      <c r="M18">
+        <v>56</v>
+      </c>
+      <c r="N18">
+        <v>4</v>
+      </c>
+      <c r="O18">
+        <v>0.37142199999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>848</v>
+      </c>
+      <c r="B19">
+        <v>80</v>
+      </c>
+      <c r="C19">
+        <v>87</v>
+      </c>
+      <c r="D19">
+        <v>7</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="G19">
+        <v>71</v>
+      </c>
+      <c r="H19">
+        <v>80</v>
+      </c>
+      <c r="I19">
+        <v>10</v>
+      </c>
+      <c r="K19" t="s">
+        <v>785</v>
+      </c>
+      <c r="L19">
+        <v>71</v>
+      </c>
+      <c r="M19">
+        <v>80</v>
+      </c>
+      <c r="N19">
+        <v>10</v>
+      </c>
+      <c r="O19">
+        <v>0.25122699999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>850</v>
+      </c>
+      <c r="B20">
+        <v>80</v>
+      </c>
+      <c r="C20">
+        <v>87</v>
+      </c>
+      <c r="D20">
+        <v>7</v>
+      </c>
+      <c r="F20" t="s">
+        <v>728</v>
+      </c>
+      <c r="G20">
+        <v>81</v>
+      </c>
+      <c r="H20">
+        <v>81</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="K20" t="s">
+        <v>786</v>
+      </c>
+      <c r="L20">
+        <v>81</v>
+      </c>
+      <c r="M20">
+        <v>81</v>
+      </c>
+      <c r="N20">
+        <v>1</v>
+      </c>
+      <c r="O20">
+        <v>5.8912399999999998E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>852</v>
+      </c>
+      <c r="B21">
+        <v>82</v>
+      </c>
+      <c r="C21">
+        <v>85</v>
+      </c>
+      <c r="D21">
+        <v>4</v>
+      </c>
+      <c r="F21" t="s">
+        <v>729</v>
+      </c>
+      <c r="G21">
+        <v>89</v>
+      </c>
+      <c r="H21">
+        <v>92</v>
+      </c>
+      <c r="I21">
+        <v>4</v>
+      </c>
+      <c r="K21" t="s">
+        <v>787</v>
+      </c>
+      <c r="L21">
+        <v>89</v>
+      </c>
+      <c r="M21">
+        <v>92</v>
+      </c>
+      <c r="N21">
+        <v>4</v>
+      </c>
+      <c r="O21">
+        <v>4.4145999999999998E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>854</v>
+      </c>
+      <c r="B22">
+        <v>85</v>
+      </c>
+      <c r="C22">
+        <v>87</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="F22" t="s">
+        <v>730</v>
+      </c>
+      <c r="G22">
+        <v>89</v>
+      </c>
+      <c r="H22">
+        <v>95</v>
+      </c>
+      <c r="I22">
+        <v>7</v>
+      </c>
+      <c r="K22" t="s">
+        <v>788</v>
+      </c>
+      <c r="L22">
+        <v>89</v>
+      </c>
+      <c r="M22">
+        <v>95</v>
+      </c>
+      <c r="N22">
+        <v>7</v>
+      </c>
+      <c r="O22">
+        <v>0.175484</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>856</v>
+      </c>
+      <c r="B23">
+        <v>87</v>
+      </c>
+      <c r="C23">
+        <v>91</v>
+      </c>
+      <c r="D23">
+        <v>5</v>
+      </c>
+      <c r="F23" t="s">
+        <v>731</v>
+      </c>
+      <c r="G23">
+        <v>95</v>
+      </c>
+      <c r="H23">
+        <v>103</v>
+      </c>
+      <c r="I23">
+        <v>9</v>
+      </c>
+      <c r="K23" t="s">
+        <v>789</v>
+      </c>
+      <c r="L23">
+        <v>95</v>
+      </c>
+      <c r="M23">
+        <v>103</v>
+      </c>
+      <c r="N23">
+        <v>9</v>
+      </c>
+      <c r="O23">
+        <v>0.25396099999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>858</v>
+      </c>
+      <c r="B24">
+        <v>94</v>
+      </c>
+      <c r="C24">
+        <v>97</v>
+      </c>
+      <c r="D24">
+        <v>4</v>
+      </c>
+      <c r="F24" t="s">
+        <v>734</v>
+      </c>
+      <c r="G24">
+        <v>88</v>
+      </c>
+      <c r="H24">
+        <v>91</v>
+      </c>
+      <c r="I24">
+        <v>4</v>
+      </c>
+      <c r="K24" t="s">
+        <v>790</v>
+      </c>
+      <c r="L24">
+        <v>88</v>
+      </c>
+      <c r="M24">
+        <v>91</v>
+      </c>
+      <c r="N24">
+        <v>4</v>
+      </c>
+      <c r="O24">
+        <v>6.2518900000000002E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>860</v>
+      </c>
+      <c r="B25">
+        <v>95</v>
+      </c>
+      <c r="C25">
+        <v>97</v>
+      </c>
+      <c r="D25">
+        <v>3</v>
+      </c>
+      <c r="F25" t="s">
+        <v>735</v>
+      </c>
+      <c r="G25">
+        <v>93</v>
+      </c>
+      <c r="H25">
+        <v>96</v>
+      </c>
+      <c r="I25">
+        <v>4</v>
+      </c>
+      <c r="K25" t="s">
+        <v>791</v>
+      </c>
+      <c r="L25">
+        <v>93</v>
+      </c>
+      <c r="M25">
+        <v>96</v>
+      </c>
+      <c r="N25">
+        <v>4</v>
+      </c>
+      <c r="O25">
+        <v>9.1641700000000006E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>862</v>
+      </c>
+      <c r="B26">
+        <v>100</v>
+      </c>
+      <c r="C26">
+        <v>105</v>
+      </c>
+      <c r="D26">
+        <v>6</v>
+      </c>
+      <c r="F26" t="s">
+        <v>738</v>
+      </c>
+      <c r="G26">
+        <v>104</v>
+      </c>
+      <c r="H26">
+        <v>104</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="K26" t="s">
+        <v>792</v>
+      </c>
+      <c r="L26">
+        <v>104</v>
+      </c>
+      <c r="M26">
+        <v>104</v>
+      </c>
+      <c r="N26">
+        <v>2</v>
+      </c>
+      <c r="O26">
+        <v>3.8808200000000001E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>864</v>
+      </c>
+      <c r="B27">
+        <v>102</v>
+      </c>
+      <c r="C27">
+        <v>110</v>
+      </c>
+      <c r="D27">
+        <v>9</v>
+      </c>
+      <c r="F27" t="s">
+        <v>739</v>
+      </c>
+      <c r="G27">
+        <v>107</v>
+      </c>
+      <c r="H27">
+        <v>117</v>
+      </c>
+      <c r="I27">
+        <v>18</v>
+      </c>
+      <c r="K27" t="s">
+        <v>793</v>
+      </c>
+      <c r="L27">
+        <v>107</v>
+      </c>
+      <c r="M27">
+        <v>117</v>
+      </c>
+      <c r="N27">
+        <v>19</v>
+      </c>
+      <c r="O27">
+        <v>0.54232000000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>866</v>
+      </c>
+      <c r="B28">
+        <v>103</v>
+      </c>
+      <c r="C28">
+        <v>109</v>
+      </c>
+      <c r="D28">
+        <v>7</v>
+      </c>
+      <c r="F28" t="s">
+        <v>740</v>
+      </c>
+      <c r="G28">
+        <v>96</v>
+      </c>
+      <c r="H28">
+        <v>98</v>
+      </c>
+      <c r="I28">
+        <v>3</v>
+      </c>
+      <c r="K28" t="s">
+        <v>794</v>
+      </c>
+      <c r="L28">
+        <v>96</v>
+      </c>
+      <c r="M28">
+        <v>98</v>
+      </c>
+      <c r="N28">
+        <v>3</v>
+      </c>
+      <c r="O28">
+        <v>4.7216800000000003E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>868</v>
+      </c>
+      <c r="B29">
+        <v>105</v>
+      </c>
+      <c r="C29">
+        <v>108</v>
+      </c>
+      <c r="D29">
+        <v>4</v>
+      </c>
+      <c r="F29" t="s">
+        <v>741</v>
+      </c>
+      <c r="G29">
+        <v>91</v>
+      </c>
+      <c r="H29">
+        <v>93</v>
+      </c>
+      <c r="I29">
+        <v>3</v>
+      </c>
+      <c r="K29" t="s">
+        <v>795</v>
+      </c>
+      <c r="L29">
+        <v>91</v>
+      </c>
+      <c r="M29">
+        <v>93</v>
+      </c>
+      <c r="N29">
+        <v>3</v>
+      </c>
+      <c r="O29">
+        <v>4.9978599999999998E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>870</v>
+      </c>
+      <c r="B30">
+        <v>107</v>
+      </c>
+      <c r="C30">
+        <v>110</v>
+      </c>
+      <c r="D30">
+        <v>4</v>
+      </c>
+      <c r="F30" t="s">
+        <v>742</v>
+      </c>
+      <c r="G30">
+        <v>111</v>
+      </c>
+      <c r="H30">
+        <v>113</v>
+      </c>
+      <c r="I30">
+        <v>3</v>
+      </c>
+      <c r="K30" t="s">
+        <v>796</v>
+      </c>
+      <c r="L30">
+        <v>111</v>
+      </c>
+      <c r="M30">
+        <v>113</v>
+      </c>
+      <c r="N30">
+        <v>3</v>
+      </c>
+      <c r="O30">
+        <v>3.87512E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>872</v>
+      </c>
+      <c r="B31">
+        <v>112</v>
+      </c>
+      <c r="C31">
+        <v>114</v>
+      </c>
+      <c r="D31">
+        <v>3</v>
+      </c>
+      <c r="F31" t="s">
+        <v>743</v>
+      </c>
+      <c r="G31">
+        <v>119</v>
+      </c>
+      <c r="H31">
+        <v>120</v>
+      </c>
+      <c r="I31">
+        <v>2</v>
+      </c>
+      <c r="K31" t="s">
+        <v>797</v>
+      </c>
+      <c r="L31">
+        <v>119</v>
+      </c>
+      <c r="M31">
+        <v>120</v>
+      </c>
+      <c r="N31">
+        <v>2</v>
+      </c>
+      <c r="O31">
+        <v>2.5018200000000001E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>874</v>
+      </c>
+      <c r="B32">
+        <v>120</v>
+      </c>
+      <c r="C32">
+        <v>124</v>
+      </c>
+      <c r="D32">
+        <v>5</v>
+      </c>
+      <c r="F32" t="s">
+        <v>746</v>
+      </c>
+      <c r="G32">
+        <v>114</v>
+      </c>
+      <c r="H32">
+        <v>116</v>
+      </c>
+      <c r="I32">
+        <v>3</v>
+      </c>
+      <c r="K32" t="s">
+        <v>798</v>
+      </c>
+      <c r="L32">
+        <v>114</v>
+      </c>
+      <c r="M32">
+        <v>116</v>
+      </c>
+      <c r="N32">
+        <v>3</v>
+      </c>
+      <c r="O32">
+        <v>3.4317399999999998E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>876</v>
+      </c>
+      <c r="B33">
+        <v>122</v>
+      </c>
+      <c r="C33">
+        <v>126</v>
+      </c>
+      <c r="D33">
+        <v>5</v>
+      </c>
+      <c r="F33" t="s">
+        <v>747</v>
+      </c>
+      <c r="G33">
+        <v>123</v>
+      </c>
+      <c r="H33">
+        <v>125</v>
+      </c>
+      <c r="I33">
+        <v>3</v>
+      </c>
+      <c r="K33" t="s">
+        <v>799</v>
+      </c>
+      <c r="L33">
+        <v>123</v>
+      </c>
+      <c r="M33">
+        <v>125</v>
+      </c>
+      <c r="N33">
+        <v>3</v>
+      </c>
+      <c r="O33">
+        <v>4.2913600000000003E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>878</v>
+      </c>
+      <c r="B34">
+        <v>122</v>
+      </c>
+      <c r="C34">
+        <v>125</v>
+      </c>
+      <c r="D34">
+        <v>4</v>
+      </c>
+      <c r="F34" t="s">
+        <v>748</v>
+      </c>
+      <c r="G34">
+        <v>120</v>
+      </c>
+      <c r="H34">
+        <v>123</v>
+      </c>
+      <c r="I34">
+        <v>4</v>
+      </c>
+      <c r="K34" t="s">
+        <v>800</v>
+      </c>
+      <c r="L34">
+        <v>120</v>
+      </c>
+      <c r="M34">
+        <v>123</v>
+      </c>
+      <c r="N34">
+        <v>4</v>
+      </c>
+      <c r="O34">
+        <v>4.5672999999999998E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>880</v>
+      </c>
+      <c r="B35">
+        <v>122</v>
+      </c>
+      <c r="C35">
+        <v>128</v>
+      </c>
+      <c r="D35">
+        <v>7</v>
+      </c>
+      <c r="F35" t="s">
+        <v>749</v>
+      </c>
+      <c r="G35">
+        <v>127</v>
+      </c>
+      <c r="H35">
+        <v>134</v>
+      </c>
+      <c r="I35">
+        <v>11</v>
+      </c>
+      <c r="K35" t="s">
+        <v>801</v>
+      </c>
+      <c r="L35">
+        <v>127</v>
+      </c>
+      <c r="M35">
+        <v>134</v>
+      </c>
+      <c r="N35">
+        <v>12</v>
+      </c>
+      <c r="O35">
+        <v>0.25062200000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>882</v>
+      </c>
+      <c r="B36">
+        <v>123</v>
+      </c>
+      <c r="C36">
+        <v>127</v>
+      </c>
+      <c r="D36">
+        <v>5</v>
+      </c>
+      <c r="F36" t="s">
+        <v>750</v>
+      </c>
+      <c r="G36">
+        <v>128</v>
+      </c>
+      <c r="H36">
+        <v>129</v>
+      </c>
+      <c r="I36">
+        <v>2</v>
+      </c>
+      <c r="K36" t="s">
+        <v>802</v>
+      </c>
+      <c r="L36">
+        <v>128</v>
+      </c>
+      <c r="M36">
+        <v>129</v>
+      </c>
+      <c r="N36">
+        <v>4</v>
+      </c>
+      <c r="O36">
+        <v>0.112335</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>884</v>
+      </c>
+      <c r="B37">
+        <v>131</v>
+      </c>
+      <c r="C37">
+        <v>134</v>
+      </c>
+      <c r="D37">
+        <v>4</v>
+      </c>
+      <c r="F37" t="s">
+        <v>751</v>
+      </c>
+      <c r="G37">
+        <v>134</v>
+      </c>
+      <c r="H37">
+        <v>136</v>
+      </c>
+      <c r="I37">
+        <v>3</v>
+      </c>
+      <c r="K37" t="s">
+        <v>803</v>
+      </c>
+      <c r="L37">
+        <v>134</v>
+      </c>
+      <c r="M37">
+        <v>136</v>
+      </c>
+      <c r="N37">
+        <v>3</v>
+      </c>
+      <c r="O37">
+        <v>2.7959299999999999E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>886</v>
+      </c>
+      <c r="B38">
+        <v>134</v>
+      </c>
+      <c r="C38">
+        <v>139</v>
+      </c>
+      <c r="D38">
+        <v>6</v>
+      </c>
+      <c r="F38" t="s">
+        <v>752</v>
+      </c>
+      <c r="G38">
+        <v>132</v>
+      </c>
+      <c r="H38">
+        <v>137</v>
+      </c>
+      <c r="I38">
+        <v>6</v>
+      </c>
+      <c r="K38" t="s">
+        <v>804</v>
+      </c>
+      <c r="L38">
+        <v>132</v>
+      </c>
+      <c r="M38">
+        <v>137</v>
+      </c>
+      <c r="N38">
+        <v>6</v>
+      </c>
+      <c r="O38">
+        <v>9.3017000000000002E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>888</v>
+      </c>
+      <c r="B39">
+        <v>144</v>
+      </c>
+      <c r="C39">
+        <v>147</v>
+      </c>
+      <c r="D39">
+        <v>4</v>
+      </c>
+      <c r="F39" t="s">
+        <v>753</v>
+      </c>
+      <c r="G39">
+        <v>148</v>
+      </c>
+      <c r="H39">
+        <v>150</v>
+      </c>
+      <c r="I39">
+        <v>3</v>
+      </c>
+      <c r="K39" t="s">
+        <v>805</v>
+      </c>
+      <c r="L39">
+        <v>148</v>
+      </c>
+      <c r="M39">
+        <v>150</v>
+      </c>
+      <c r="N39">
+        <v>3</v>
+      </c>
+      <c r="O39">
+        <v>2.9907799999999998E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>890</v>
+      </c>
+      <c r="B40">
+        <v>151</v>
+      </c>
+      <c r="C40">
+        <v>152</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
+      <c r="F40" t="s">
+        <v>757</v>
+      </c>
+      <c r="G40">
+        <v>135</v>
+      </c>
+      <c r="H40">
+        <v>136</v>
+      </c>
+      <c r="I40">
+        <v>2</v>
+      </c>
+      <c r="K40" t="s">
+        <v>806</v>
+      </c>
+      <c r="L40">
+        <v>135</v>
+      </c>
+      <c r="M40">
+        <v>136</v>
+      </c>
+      <c r="N40">
+        <v>3</v>
+      </c>
+      <c r="O40">
+        <v>3.70341E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>892</v>
+      </c>
+      <c r="B41">
+        <v>153</v>
+      </c>
+      <c r="C41">
+        <v>156</v>
+      </c>
+      <c r="D41">
+        <v>4</v>
+      </c>
+      <c r="F41" t="s">
+        <v>758</v>
+      </c>
+      <c r="G41">
+        <v>156</v>
+      </c>
+      <c r="H41">
+        <v>157</v>
+      </c>
+      <c r="I41">
+        <v>2</v>
+      </c>
+      <c r="K41" t="s">
+        <v>807</v>
+      </c>
+      <c r="L41">
+        <v>156</v>
+      </c>
+      <c r="M41">
+        <v>157</v>
+      </c>
+      <c r="N41">
+        <v>2</v>
+      </c>
+      <c r="O41">
+        <v>3.1209600000000001E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>894</v>
+      </c>
+      <c r="B42">
+        <v>156</v>
+      </c>
+      <c r="C42">
+        <v>159</v>
+      </c>
+      <c r="D42">
+        <v>4</v>
+      </c>
+      <c r="F42" t="s">
+        <v>759</v>
+      </c>
+      <c r="G42">
+        <v>157</v>
+      </c>
+      <c r="H42">
+        <v>160</v>
+      </c>
+      <c r="I42">
+        <v>4</v>
+      </c>
+      <c r="K42" t="s">
+        <v>808</v>
+      </c>
+      <c r="L42">
+        <v>157</v>
+      </c>
+      <c r="M42">
+        <v>160</v>
+      </c>
+      <c r="N42">
+        <v>4</v>
+      </c>
+      <c r="O42">
+        <v>5.0618900000000001E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>896</v>
+      </c>
+      <c r="B43">
+        <v>158</v>
+      </c>
+      <c r="C43">
+        <v>163</v>
+      </c>
+      <c r="D43">
+        <v>6</v>
+      </c>
+      <c r="F43" t="s">
+        <v>760</v>
+      </c>
+      <c r="G43">
+        <v>148</v>
+      </c>
+      <c r="H43">
+        <v>155</v>
+      </c>
+      <c r="I43">
+        <v>10</v>
+      </c>
+      <c r="K43" t="s">
+        <v>809</v>
+      </c>
+      <c r="L43">
+        <v>148</v>
+      </c>
+      <c r="M43">
+        <v>155</v>
+      </c>
+      <c r="N43">
+        <v>12</v>
+      </c>
+      <c r="O43">
+        <v>0.41206100000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>898</v>
+      </c>
+      <c r="B44">
+        <v>160</v>
+      </c>
+      <c r="C44">
+        <v>166</v>
+      </c>
+      <c r="D44">
+        <v>7</v>
+      </c>
+      <c r="F44" t="s">
+        <v>761</v>
+      </c>
+      <c r="G44">
+        <v>148</v>
+      </c>
+      <c r="H44">
+        <v>155</v>
+      </c>
+      <c r="I44">
+        <v>8</v>
+      </c>
+      <c r="K44" t="s">
+        <v>810</v>
+      </c>
+      <c r="L44">
+        <v>148</v>
+      </c>
+      <c r="M44">
+        <v>155</v>
+      </c>
+      <c r="N44">
+        <v>8</v>
+      </c>
+      <c r="O44">
+        <v>0.170097</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>900</v>
+      </c>
+      <c r="B45">
+        <v>160</v>
+      </c>
+      <c r="C45">
+        <v>166</v>
+      </c>
+      <c r="D45">
+        <v>5</v>
+      </c>
+      <c r="F45" t="s">
+        <v>762</v>
+      </c>
+      <c r="G45">
+        <v>161</v>
+      </c>
+      <c r="H45">
+        <v>164</v>
+      </c>
+      <c r="I45">
+        <v>4</v>
+      </c>
+      <c r="K45" t="s">
+        <v>811</v>
+      </c>
+      <c r="L45">
+        <v>161</v>
+      </c>
+      <c r="M45">
+        <v>164</v>
+      </c>
+      <c r="N45">
+        <v>4</v>
+      </c>
+      <c r="O45">
+        <v>7.0787100000000006E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>902</v>
+      </c>
+      <c r="B46">
+        <v>163</v>
+      </c>
+      <c r="C46">
+        <v>167</v>
+      </c>
+      <c r="D46">
+        <v>5</v>
+      </c>
+      <c r="F46" t="s">
+        <v>763</v>
+      </c>
+      <c r="G46">
+        <v>181</v>
+      </c>
+      <c r="H46">
+        <v>182</v>
+      </c>
+      <c r="I46">
+        <v>2</v>
+      </c>
+      <c r="K46" t="s">
+        <v>812</v>
+      </c>
+      <c r="L46">
+        <v>181</v>
+      </c>
+      <c r="M46">
+        <v>182</v>
+      </c>
+      <c r="N46">
+        <v>2</v>
+      </c>
+      <c r="O46">
+        <v>2.4920100000000001E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>904</v>
+      </c>
+      <c r="B47">
+        <v>173</v>
+      </c>
+      <c r="C47">
+        <v>178</v>
+      </c>
+      <c r="D47">
+        <v>6</v>
+      </c>
+      <c r="F47" t="s">
+        <v>764</v>
+      </c>
+      <c r="G47">
+        <v>186</v>
+      </c>
+      <c r="H47">
+        <v>190</v>
+      </c>
+      <c r="I47">
+        <v>5</v>
+      </c>
+      <c r="K47" t="s">
+        <v>813</v>
+      </c>
+      <c r="L47">
+        <v>186</v>
+      </c>
+      <c r="M47">
+        <v>190</v>
+      </c>
+      <c r="N47">
+        <v>5</v>
+      </c>
+      <c r="O47">
+        <v>6.4135999999999999E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>906</v>
+      </c>
+      <c r="B48">
+        <v>181</v>
+      </c>
+      <c r="C48">
+        <v>188</v>
+      </c>
+      <c r="D48">
+        <v>8</v>
+      </c>
+      <c r="F48" t="s">
+        <v>765</v>
+      </c>
+      <c r="G48">
+        <v>189</v>
+      </c>
+      <c r="H48">
+        <v>197</v>
+      </c>
+      <c r="I48">
+        <v>9</v>
+      </c>
+      <c r="K48" t="s">
+        <v>814</v>
+      </c>
+      <c r="L48">
+        <v>189</v>
+      </c>
+      <c r="M48">
+        <v>194</v>
+      </c>
+      <c r="N48">
+        <v>6</v>
+      </c>
+      <c r="O48">
+        <v>0.115923</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>908</v>
+      </c>
+      <c r="B49">
+        <v>196</v>
+      </c>
+      <c r="C49">
+        <v>201</v>
+      </c>
+      <c r="D49">
+        <v>6</v>
+      </c>
+      <c r="F49" s="2"/>
+      <c r="K49" t="s">
+        <v>815</v>
+      </c>
+      <c r="L49">
+        <v>195</v>
+      </c>
+      <c r="M49">
+        <v>197</v>
+      </c>
+      <c r="N49">
+        <v>3</v>
+      </c>
+      <c r="O49">
+        <v>4.5745500000000001E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>910</v>
+      </c>
+      <c r="B50">
+        <v>204</v>
+      </c>
+      <c r="C50">
+        <v>204</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{739C6FA6-EA7C-4018-8DB3-BD76C74CF2D4}">
+  <dimension ref="A1:W37"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:O37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S1" t="s">
+        <v>2</v>
+      </c>
+      <c r="T1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U1" t="s">
+        <v>4</v>
+      </c>
+      <c r="V1" t="s">
+        <v>5</v>
+      </c>
+      <c r="W1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1503</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>14</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1406</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>4</v>
+      </c>
+      <c r="I2">
+        <v>4</v>
+      </c>
+      <c r="K2" t="s">
+        <v>1454</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>4</v>
+      </c>
+      <c r="N2">
+        <v>4</v>
+      </c>
+      <c r="O2">
+        <v>4.6210800000000003E-2</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>1310</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>210</v>
+      </c>
+      <c r="T2">
+        <v>520</v>
+      </c>
+      <c r="U2">
+        <v>64.3245</v>
+      </c>
+      <c r="V2">
+        <v>159.15199999999999</v>
+      </c>
+      <c r="W2">
+        <v>9.8673900000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B3">
+        <v>18</v>
+      </c>
+      <c r="C3">
+        <v>23</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1452</v>
+      </c>
+      <c r="G3">
+        <v>18</v>
+      </c>
+      <c r="H3">
+        <v>23</v>
+      </c>
+      <c r="I3">
+        <v>6</v>
+      </c>
+      <c r="K3" t="s">
+        <v>1487</v>
+      </c>
+      <c r="L3">
+        <v>18</v>
+      </c>
+      <c r="M3">
+        <v>23</v>
+      </c>
+      <c r="N3">
+        <v>6</v>
+      </c>
+      <c r="O3">
+        <v>8.4451499999999999E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1505</v>
+      </c>
+      <c r="B4">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>26</v>
+      </c>
+      <c r="D4">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1407</v>
+      </c>
+      <c r="G4">
+        <v>17</v>
+      </c>
+      <c r="H4">
+        <v>21</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="K4" t="s">
+        <v>1455</v>
+      </c>
+      <c r="L4">
+        <v>17</v>
+      </c>
+      <c r="M4">
+        <v>21</v>
+      </c>
+      <c r="N4">
+        <v>5</v>
+      </c>
+      <c r="O4">
+        <v>6.2676399999999993E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1507</v>
+      </c>
+      <c r="B5">
+        <v>35</v>
+      </c>
+      <c r="C5">
+        <v>38</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1408</v>
+      </c>
+      <c r="G5">
+        <v>22</v>
+      </c>
+      <c r="H5">
+        <v>33</v>
+      </c>
+      <c r="I5">
+        <v>14</v>
+      </c>
+      <c r="K5" t="s">
+        <v>1456</v>
+      </c>
+      <c r="L5">
+        <v>22</v>
+      </c>
+      <c r="M5">
+        <v>33</v>
+      </c>
+      <c r="N5">
+        <v>14</v>
+      </c>
+      <c r="O5">
+        <v>0.390567</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1509</v>
+      </c>
+      <c r="B6">
+        <v>39</v>
+      </c>
+      <c r="C6">
+        <v>43</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1409</v>
+      </c>
+      <c r="G6">
+        <v>49</v>
+      </c>
+      <c r="H6">
+        <v>52</v>
+      </c>
+      <c r="I6">
+        <v>4</v>
+      </c>
+      <c r="K6" t="s">
+        <v>1457</v>
+      </c>
+      <c r="L6">
+        <v>49</v>
+      </c>
+      <c r="M6">
+        <v>52</v>
+      </c>
+      <c r="N6">
+        <v>5</v>
+      </c>
+      <c r="O6">
+        <v>6.2744300000000003E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1511</v>
+      </c>
+      <c r="B7">
+        <v>40</v>
+      </c>
+      <c r="C7">
+        <v>44</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1410</v>
+      </c>
+      <c r="G7">
+        <v>43</v>
+      </c>
+      <c r="H7">
+        <v>45</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
+      <c r="K7" t="s">
+        <v>1458</v>
+      </c>
+      <c r="L7">
+        <v>43</v>
+      </c>
+      <c r="M7">
+        <v>45</v>
+      </c>
+      <c r="N7">
+        <v>4</v>
+      </c>
+      <c r="O7">
+        <v>8.1246100000000002E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1513</v>
+      </c>
+      <c r="B8">
+        <v>42</v>
+      </c>
+      <c r="C8">
+        <v>47</v>
+      </c>
+      <c r="D8">
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G8">
+        <v>36</v>
+      </c>
+      <c r="H8">
+        <v>37</v>
+      </c>
+      <c r="I8">
+        <v>2</v>
+      </c>
+      <c r="K8" t="s">
+        <v>1459</v>
+      </c>
+      <c r="L8">
+        <v>36</v>
+      </c>
+      <c r="M8">
+        <v>37</v>
+      </c>
+      <c r="N8">
+        <v>4</v>
+      </c>
+      <c r="O8">
+        <v>5.19067E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1515</v>
+      </c>
+      <c r="B9">
+        <v>51</v>
+      </c>
+      <c r="C9">
+        <v>55</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1412</v>
+      </c>
+      <c r="G9">
+        <v>44</v>
+      </c>
+      <c r="H9">
+        <v>46</v>
+      </c>
+      <c r="I9">
+        <v>3</v>
+      </c>
+      <c r="K9" t="s">
+        <v>1460</v>
+      </c>
+      <c r="L9">
+        <v>44</v>
+      </c>
+      <c r="M9">
+        <v>46</v>
+      </c>
+      <c r="N9">
+        <v>3</v>
+      </c>
+      <c r="O9">
+        <v>3.8751899999999999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1517</v>
+      </c>
+      <c r="B10">
+        <v>53</v>
+      </c>
+      <c r="C10">
+        <v>56</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1413</v>
+      </c>
+      <c r="G10">
+        <v>49</v>
+      </c>
+      <c r="H10">
+        <v>58</v>
+      </c>
+      <c r="I10">
+        <v>11</v>
+      </c>
+      <c r="K10" t="s">
+        <v>1461</v>
+      </c>
+      <c r="L10">
+        <v>49</v>
+      </c>
+      <c r="M10">
+        <v>58</v>
+      </c>
+      <c r="N10">
+        <v>11</v>
+      </c>
+      <c r="O10">
+        <v>0.34978199999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1519</v>
+      </c>
+      <c r="B11">
+        <v>54</v>
+      </c>
+      <c r="C11">
+        <v>56</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1414</v>
+      </c>
+      <c r="G11">
+        <v>43</v>
+      </c>
+      <c r="H11">
+        <v>45</v>
+      </c>
+      <c r="I11">
+        <v>3</v>
+      </c>
+      <c r="K11" t="s">
+        <v>1462</v>
+      </c>
+      <c r="L11">
+        <v>43</v>
+      </c>
+      <c r="M11">
+        <v>45</v>
+      </c>
+      <c r="N11">
+        <v>3</v>
+      </c>
+      <c r="O11">
+        <v>3.9679600000000002E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1521</v>
+      </c>
+      <c r="B12">
+        <v>59</v>
+      </c>
+      <c r="C12">
+        <v>66</v>
+      </c>
+      <c r="D12">
+        <v>8</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1415</v>
+      </c>
+      <c r="G12">
+        <v>60</v>
+      </c>
+      <c r="H12">
+        <v>64</v>
+      </c>
+      <c r="I12">
+        <v>5</v>
+      </c>
+      <c r="K12" t="s">
+        <v>1463</v>
+      </c>
+      <c r="L12">
+        <v>60</v>
+      </c>
+      <c r="M12">
+        <v>64</v>
+      </c>
+      <c r="N12">
+        <v>5</v>
+      </c>
+      <c r="O12">
+        <v>8.8473899999999994E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1523</v>
+      </c>
+      <c r="B13">
+        <v>66</v>
+      </c>
+      <c r="C13">
+        <v>71</v>
+      </c>
+      <c r="D13">
+        <v>6</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1416</v>
+      </c>
+      <c r="G13">
+        <v>87</v>
+      </c>
+      <c r="H13">
+        <v>88</v>
+      </c>
+      <c r="I13">
+        <v>2</v>
+      </c>
+      <c r="K13" t="s">
+        <v>1464</v>
+      </c>
+      <c r="L13">
+        <v>87</v>
+      </c>
+      <c r="M13">
+        <v>88</v>
+      </c>
+      <c r="N13">
+        <v>3</v>
+      </c>
+      <c r="O13">
+        <v>3.64699E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1525</v>
+      </c>
+      <c r="B14">
+        <v>79</v>
+      </c>
+      <c r="C14">
+        <v>82</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1417</v>
+      </c>
+      <c r="G14">
+        <v>72</v>
+      </c>
+      <c r="H14">
+        <v>78</v>
+      </c>
+      <c r="I14">
+        <v>7</v>
+      </c>
+      <c r="K14" t="s">
+        <v>1465</v>
+      </c>
+      <c r="L14">
+        <v>72</v>
+      </c>
+      <c r="M14">
+        <v>78</v>
+      </c>
+      <c r="N14">
+        <v>7</v>
+      </c>
+      <c r="O14">
+        <v>9.18881E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1573</v>
+      </c>
+      <c r="B15">
+        <v>85</v>
+      </c>
+      <c r="C15">
+        <v>87</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="F15" t="s">
+        <v>1453</v>
+      </c>
+      <c r="G15">
+        <v>85</v>
+      </c>
+      <c r="H15">
+        <v>92</v>
+      </c>
+      <c r="I15">
+        <v>8</v>
+      </c>
+      <c r="K15" t="s">
+        <v>1488</v>
+      </c>
+      <c r="L15">
+        <v>85</v>
+      </c>
+      <c r="M15">
+        <v>92</v>
+      </c>
+      <c r="N15">
+        <v>8</v>
+      </c>
+      <c r="O15">
+        <v>0.14616199999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1527</v>
+      </c>
+      <c r="B16">
+        <v>88</v>
+      </c>
+      <c r="C16">
+        <v>94</v>
+      </c>
+      <c r="D16">
+        <v>7</v>
+      </c>
+      <c r="F16" t="s">
+        <v>1418</v>
+      </c>
+      <c r="G16">
+        <v>89</v>
+      </c>
+      <c r="H16">
+        <v>93</v>
+      </c>
+      <c r="I16">
+        <v>5</v>
+      </c>
+      <c r="K16" t="s">
+        <v>1466</v>
+      </c>
+      <c r="L16">
+        <v>89</v>
+      </c>
+      <c r="M16">
+        <v>93</v>
+      </c>
+      <c r="N16">
+        <v>5</v>
+      </c>
+      <c r="O16">
+        <v>0.10907799999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>1529</v>
+      </c>
+      <c r="B17">
+        <v>92</v>
+      </c>
+      <c r="C17">
+        <v>97</v>
+      </c>
+      <c r="D17">
+        <v>6</v>
+      </c>
+      <c r="F17" t="s">
+        <v>1421</v>
+      </c>
+      <c r="G17">
+        <v>92</v>
+      </c>
+      <c r="H17">
+        <v>97</v>
+      </c>
+      <c r="I17">
+        <v>6</v>
+      </c>
+      <c r="K17" t="s">
+        <v>1467</v>
+      </c>
+      <c r="L17">
+        <v>92</v>
+      </c>
+      <c r="M17">
+        <v>97</v>
+      </c>
+      <c r="N17">
+        <v>6</v>
+      </c>
+      <c r="O17">
+        <v>0.128193</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1530</v>
+      </c>
+      <c r="B18">
+        <v>94</v>
+      </c>
+      <c r="C18">
+        <v>96</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="F18" t="s">
+        <v>1422</v>
+      </c>
+      <c r="G18">
+        <v>110</v>
+      </c>
+      <c r="H18">
+        <v>113</v>
+      </c>
+      <c r="I18">
+        <v>4</v>
+      </c>
+      <c r="K18" t="s">
+        <v>1468</v>
+      </c>
+      <c r="L18">
+        <v>110</v>
+      </c>
+      <c r="M18">
+        <v>113</v>
+      </c>
+      <c r="N18">
+        <v>4</v>
+      </c>
+      <c r="O18">
+        <v>5.3845200000000003E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1532</v>
+      </c>
+      <c r="B19">
+        <v>97</v>
+      </c>
+      <c r="C19">
+        <v>101</v>
+      </c>
+      <c r="D19">
+        <v>5</v>
+      </c>
+      <c r="F19" t="s">
+        <v>1423</v>
+      </c>
+      <c r="G19">
+        <v>96</v>
+      </c>
+      <c r="H19">
+        <v>105</v>
+      </c>
+      <c r="I19">
+        <v>10</v>
+      </c>
+      <c r="K19" t="s">
+        <v>1469</v>
+      </c>
+      <c r="L19">
+        <v>96</v>
+      </c>
+      <c r="M19">
+        <v>105</v>
+      </c>
+      <c r="N19">
+        <v>10</v>
+      </c>
+      <c r="O19">
+        <v>0.225243</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>1534</v>
+      </c>
+      <c r="B20">
+        <v>102</v>
+      </c>
+      <c r="C20">
+        <v>108</v>
+      </c>
+      <c r="D20">
+        <v>7</v>
+      </c>
+      <c r="F20" t="s">
+        <v>1424</v>
+      </c>
+      <c r="G20">
+        <v>101</v>
+      </c>
+      <c r="H20">
+        <v>105</v>
+      </c>
+      <c r="I20">
+        <v>5</v>
+      </c>
+      <c r="K20" t="s">
+        <v>1470</v>
+      </c>
+      <c r="L20">
+        <v>101</v>
+      </c>
+      <c r="M20">
+        <v>105</v>
+      </c>
+      <c r="N20">
+        <v>5</v>
+      </c>
+      <c r="O20">
+        <v>7.2291499999999995E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>1536</v>
+      </c>
+      <c r="B21">
+        <v>105</v>
+      </c>
+      <c r="C21">
+        <v>107</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="F21" t="s">
+        <v>1425</v>
+      </c>
+      <c r="G21">
+        <v>91</v>
+      </c>
+      <c r="H21">
+        <v>96</v>
+      </c>
+      <c r="I21">
+        <v>6</v>
+      </c>
+      <c r="K21" t="s">
+        <v>1471</v>
+      </c>
+      <c r="L21">
+        <v>91</v>
+      </c>
+      <c r="M21">
+        <v>96</v>
+      </c>
+      <c r="N21">
+        <v>6</v>
+      </c>
+      <c r="O21">
+        <v>0.13366900000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>1538</v>
+      </c>
+      <c r="B22">
+        <v>117</v>
+      </c>
+      <c r="C22">
+        <v>120</v>
+      </c>
+      <c r="D22">
+        <v>4</v>
+      </c>
+      <c r="F22" t="s">
+        <v>1429</v>
+      </c>
+      <c r="G22">
+        <v>113</v>
+      </c>
+      <c r="H22">
+        <v>114</v>
+      </c>
+      <c r="I22">
+        <v>2</v>
+      </c>
+      <c r="K22" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L22">
+        <v>113</v>
+      </c>
+      <c r="M22">
+        <v>114</v>
+      </c>
+      <c r="N22">
+        <v>2</v>
+      </c>
+      <c r="O22">
+        <v>3.1109999999999999E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>1540</v>
+      </c>
+      <c r="B23">
+        <v>120</v>
+      </c>
+      <c r="C23">
+        <v>126</v>
+      </c>
+      <c r="D23">
+        <v>7</v>
+      </c>
+      <c r="F23" t="s">
+        <v>1430</v>
+      </c>
+      <c r="G23">
+        <v>109</v>
+      </c>
+      <c r="H23">
+        <v>112</v>
+      </c>
+      <c r="I23">
+        <v>4</v>
+      </c>
+      <c r="K23" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L23">
+        <v>109</v>
+      </c>
+      <c r="M23">
+        <v>112</v>
+      </c>
+      <c r="N23">
+        <v>5</v>
+      </c>
+      <c r="O23">
+        <v>0.116437</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>1542</v>
+      </c>
+      <c r="B24">
+        <v>128</v>
+      </c>
+      <c r="C24">
+        <v>134</v>
+      </c>
+      <c r="D24">
+        <v>7</v>
+      </c>
+      <c r="F24" t="s">
+        <v>1431</v>
+      </c>
+      <c r="G24">
+        <v>113</v>
+      </c>
+      <c r="H24">
+        <v>118</v>
+      </c>
+      <c r="I24">
+        <v>6</v>
+      </c>
+      <c r="K24" t="s">
+        <v>1474</v>
+      </c>
+      <c r="L24">
+        <v>113</v>
+      </c>
+      <c r="M24">
+        <v>118</v>
+      </c>
+      <c r="N24">
+        <v>6</v>
+      </c>
+      <c r="O24">
+        <v>0.14421</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>1544</v>
+      </c>
+      <c r="B25">
+        <v>132</v>
+      </c>
+      <c r="C25">
+        <v>136</v>
+      </c>
+      <c r="D25">
+        <v>5</v>
+      </c>
+      <c r="F25" t="s">
+        <v>1432</v>
+      </c>
+      <c r="G25">
+        <v>133</v>
+      </c>
+      <c r="H25">
+        <v>137</v>
+      </c>
+      <c r="I25">
+        <v>5</v>
+      </c>
+      <c r="K25" t="s">
+        <v>1475</v>
+      </c>
+      <c r="L25">
+        <v>133</v>
+      </c>
+      <c r="M25">
+        <v>137</v>
+      </c>
+      <c r="N25">
+        <v>5</v>
+      </c>
+      <c r="O25">
+        <v>0.101396</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>1550</v>
+      </c>
+      <c r="B26">
+        <v>140</v>
+      </c>
+      <c r="C26">
+        <v>144</v>
+      </c>
+      <c r="D26">
+        <v>5</v>
+      </c>
+      <c r="F26" t="s">
+        <v>1434</v>
+      </c>
+      <c r="G26">
+        <v>154</v>
+      </c>
+      <c r="H26">
+        <v>156</v>
+      </c>
+      <c r="I26">
+        <v>3</v>
+      </c>
+      <c r="K26" t="s">
+        <v>1477</v>
+      </c>
+      <c r="L26">
+        <v>154</v>
+      </c>
+      <c r="M26">
+        <v>155</v>
+      </c>
+      <c r="N26">
+        <v>2</v>
+      </c>
+      <c r="O26">
+        <v>1.3761900000000001E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>1546</v>
+      </c>
+      <c r="B27">
+        <v>142</v>
+      </c>
+      <c r="C27">
+        <v>148</v>
+      </c>
+      <c r="D27">
+        <v>7</v>
+      </c>
+      <c r="F27" t="s">
+        <v>1433</v>
+      </c>
+      <c r="G27">
+        <v>143</v>
+      </c>
+      <c r="H27">
+        <v>146</v>
+      </c>
+      <c r="I27">
+        <v>4</v>
+      </c>
+      <c r="K27" t="s">
+        <v>1476</v>
+      </c>
+      <c r="L27">
+        <v>143</v>
+      </c>
+      <c r="M27">
+        <v>146</v>
+      </c>
+      <c r="N27">
+        <v>4</v>
+      </c>
+      <c r="O27">
+        <v>5.5525100000000001E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>1552</v>
+      </c>
+      <c r="B28">
+        <v>145</v>
+      </c>
+      <c r="C28">
+        <v>150</v>
+      </c>
+      <c r="D28">
+        <v>6</v>
+      </c>
+      <c r="F28" t="s">
+        <v>1435</v>
+      </c>
+      <c r="G28">
+        <v>139</v>
+      </c>
+      <c r="H28">
+        <v>151</v>
+      </c>
+      <c r="I28">
+        <v>18</v>
+      </c>
+      <c r="K28" t="s">
+        <v>1478</v>
+      </c>
+      <c r="L28">
+        <v>139</v>
+      </c>
+      <c r="M28">
+        <v>151</v>
+      </c>
+      <c r="N28">
+        <v>15</v>
+      </c>
+      <c r="O28">
+        <v>0.392764</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>1554</v>
+      </c>
+      <c r="B29">
+        <v>150</v>
+      </c>
+      <c r="C29">
+        <v>153</v>
+      </c>
+      <c r="D29">
+        <v>4</v>
+      </c>
+      <c r="F29" t="s">
+        <v>1440</v>
+      </c>
+      <c r="G29">
+        <v>143</v>
+      </c>
+      <c r="H29">
+        <v>145</v>
+      </c>
+      <c r="I29">
+        <v>3</v>
+      </c>
+      <c r="K29" t="s">
+        <v>1479</v>
+      </c>
+      <c r="L29">
+        <v>143</v>
+      </c>
+      <c r="M29">
+        <v>145</v>
+      </c>
+      <c r="N29">
+        <v>3</v>
+      </c>
+      <c r="O29">
+        <v>4.4546700000000002E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>1556</v>
+      </c>
+      <c r="B30">
+        <v>151</v>
+      </c>
+      <c r="C30">
+        <v>154</v>
+      </c>
+      <c r="D30">
+        <v>4</v>
+      </c>
+      <c r="F30" t="s">
+        <v>1441</v>
+      </c>
+      <c r="G30">
+        <v>138</v>
+      </c>
+      <c r="H30">
+        <v>142</v>
+      </c>
+      <c r="I30">
+        <v>5</v>
+      </c>
+      <c r="K30" t="s">
+        <v>1480</v>
+      </c>
+      <c r="L30">
+        <v>138</v>
+      </c>
+      <c r="M30">
+        <v>142</v>
+      </c>
+      <c r="N30">
+        <v>5</v>
+      </c>
+      <c r="O30">
+        <v>6.9467399999999999E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>1559</v>
+      </c>
+      <c r="B31">
+        <v>163</v>
+      </c>
+      <c r="C31">
+        <v>166</v>
+      </c>
+      <c r="D31">
+        <v>4</v>
+      </c>
+      <c r="F31" t="s">
+        <v>1443</v>
+      </c>
+      <c r="G31">
+        <v>179</v>
+      </c>
+      <c r="H31">
+        <v>180</v>
+      </c>
+      <c r="I31">
+        <v>2</v>
+      </c>
+      <c r="K31" t="s">
+        <v>1481</v>
+      </c>
+      <c r="L31">
+        <v>179</v>
+      </c>
+      <c r="M31">
+        <v>180</v>
+      </c>
+      <c r="N31">
+        <v>4</v>
+      </c>
+      <c r="O31">
+        <v>6.7106700000000005E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>1561</v>
+      </c>
+      <c r="B32">
+        <v>166</v>
+      </c>
+      <c r="C32">
+        <v>172</v>
+      </c>
+      <c r="D32">
+        <v>7</v>
+      </c>
+      <c r="F32" t="s">
+        <v>1444</v>
+      </c>
+      <c r="G32">
+        <v>163</v>
+      </c>
+      <c r="H32">
+        <v>167</v>
+      </c>
+      <c r="I32">
+        <v>5</v>
+      </c>
+      <c r="K32" t="s">
+        <v>1482</v>
+      </c>
+      <c r="L32">
+        <v>163</v>
+      </c>
+      <c r="M32">
+        <v>167</v>
+      </c>
+      <c r="N32">
+        <v>5</v>
+      </c>
+      <c r="O32">
+        <v>6.0366799999999998E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>1563</v>
+      </c>
+      <c r="B33">
+        <v>168</v>
+      </c>
+      <c r="C33">
+        <v>173</v>
+      </c>
+      <c r="D33">
+        <v>6</v>
+      </c>
+      <c r="F33" t="s">
+        <v>1445</v>
+      </c>
+      <c r="G33">
+        <v>154</v>
+      </c>
+      <c r="H33">
+        <v>169</v>
+      </c>
+      <c r="I33">
+        <v>19</v>
+      </c>
+      <c r="K33" t="s">
+        <v>1483</v>
+      </c>
+      <c r="L33">
+        <v>154</v>
+      </c>
+      <c r="M33">
+        <v>169</v>
+      </c>
+      <c r="N33">
+        <v>19</v>
+      </c>
+      <c r="O33">
+        <v>0.68526500000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>1565</v>
+      </c>
+      <c r="B34">
+        <v>181</v>
+      </c>
+      <c r="C34">
+        <v>184</v>
+      </c>
+      <c r="D34">
+        <v>4</v>
+      </c>
+      <c r="F34" t="s">
+        <v>1449</v>
+      </c>
+      <c r="G34">
+        <v>191</v>
+      </c>
+      <c r="H34">
+        <v>193</v>
+      </c>
+      <c r="I34">
+        <v>3</v>
+      </c>
+      <c r="K34" t="s">
+        <v>1484</v>
+      </c>
+      <c r="L34">
+        <v>191</v>
+      </c>
+      <c r="M34">
+        <v>193</v>
+      </c>
+      <c r="N34">
+        <v>4</v>
+      </c>
+      <c r="O34">
+        <v>6.4546699999999999E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>1567</v>
+      </c>
+      <c r="B35">
+        <v>191</v>
+      </c>
+      <c r="C35">
+        <v>194</v>
+      </c>
+      <c r="D35">
+        <v>4</v>
+      </c>
+      <c r="F35" t="s">
+        <v>1450</v>
+      </c>
+      <c r="G35">
+        <v>187</v>
+      </c>
+      <c r="H35">
+        <v>188</v>
+      </c>
+      <c r="I35">
+        <v>2</v>
+      </c>
+      <c r="K35" t="s">
+        <v>1485</v>
+      </c>
+      <c r="L35">
+        <v>187</v>
+      </c>
+      <c r="M35">
+        <v>188</v>
+      </c>
+      <c r="N35">
+        <v>4</v>
+      </c>
+      <c r="O35">
+        <v>2.7993000000000001E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>1569</v>
+      </c>
+      <c r="B36">
+        <v>203</v>
+      </c>
+      <c r="C36">
+        <v>206</v>
+      </c>
+      <c r="D36">
+        <v>4</v>
+      </c>
+      <c r="F36" t="s">
+        <v>1451</v>
+      </c>
+      <c r="G36">
+        <v>203</v>
+      </c>
+      <c r="H36">
+        <v>207</v>
+      </c>
+      <c r="I36">
+        <v>5</v>
+      </c>
+      <c r="K36" t="s">
+        <v>1486</v>
+      </c>
+      <c r="L36">
+        <v>203</v>
+      </c>
+      <c r="M36">
+        <v>207</v>
+      </c>
+      <c r="N36">
+        <v>5</v>
+      </c>
+      <c r="O36">
+        <v>5.4580999999999998E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>1571</v>
+      </c>
+      <c r="B37">
+        <v>206</v>
+      </c>
+      <c r="C37">
+        <v>206</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D36">
+    <sortCondition ref="B2"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>